<commit_message>
Added Csv Modal Component with sampleFile
</commit_message>
<xml_diff>
--- a/client/src/assets/sampleFile.xlsx
+++ b/client/src/assets/sampleFile.xlsx
@@ -11,33 +11,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Emp id</t>
-  </si>
-  <si>
-    <t>designatin</t>
-  </si>
-  <si>
-    <t>emial</t>
-  </si>
-  <si>
-    <t>joining date</t>
-  </si>
-  <si>
-    <t>manager Name</t>
-  </si>
-  <si>
-    <t>namager email</t>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Manager Name</t>
+  </si>
+  <si>
+    <t>Manager Email</t>
+  </si>
+  <si>
+    <t>Joining Date</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>xyz@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -65,11 +89,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -310,6 +337,36 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12322.0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2">
+        <v>45292.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>